<commit_message>
Rankings file re-generated after changes to data loading
</commit_message>
<xml_diff>
--- a/Rankings_RCP45_Year2026.xlsx
+++ b/Rankings_RCP45_Year2026.xlsx
@@ -13,7 +13,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>sites_after_filtering</t>
+  </si>
+  <si>
+    <t>siteranks_alg1</t>
+  </si>
+  <si>
+    <t>siteranks_alg2</t>
+  </si>
+  <si>
+    <t>siteranks_alg3</t>
+  </si>
   <si>
     <t>sites_after_filtering</t>
   </si>
@@ -45,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -54,13 +66,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -81,16 +95,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Final data from IPMF runs
</commit_message>
<xml_diff>
--- a/Rankings_RCP45_Year2026.xlsx
+++ b/Rankings_RCP45_Year2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrocker\Documents\GitHub\ADRIA_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC788BF5-EC2A-4488-BA9A-F504A8999C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A2C578-C9F4-4364-A0DA-89BD8A0E0C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="876" windowWidth="19872" windowHeight="11628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="732" windowWidth="19872" windowHeight="11628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>sites_after_filtering</t>
+    <t>TOPSIS site ranks</t>
   </si>
   <si>
-    <t>siteranks_alg1</t>
+    <t>VIKOR site ranks</t>
   </si>
   <si>
-    <t>siteranks_alg2</t>
+    <t>Site IDs after depth filtering</t>
   </si>
   <si>
-    <t>siteranks_alg3</t>
+    <t>OR site ranks</t>
   </si>
 </sst>
 </file>
@@ -190,10 +190,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Column 1, s</a:t>
+            <a:t>Column 1</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-AU" sz="1100" i="1">
+            <a:rPr lang="en-AU" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -202,7 +202,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ites_after_filtering</a:t>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100">
@@ -214,7 +214,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>, gives the ordered site IDs following depth filtering.</a:t>
+            <a:t>gives the ordered site IDs following depth filtering.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -222,18 +222,6 @@
             <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:buChar char="•"/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" i="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>siteranks_alg1, siteranks_alg2 </a:t>
-          </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100">
               <a:solidFill>
@@ -244,10 +232,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>and </a:t>
+            <a:t>Columns</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-AU" sz="1100" i="1">
+            <a:rPr lang="en-AU" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -256,7 +244,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>siteranks_alg3 </a:t>
+            <a:t> 2,3 and 4 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100">
@@ -365,6 +353,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AFDDA301-E507-4CEA-B648-D07EEDB19C6A}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0">
+  <autoFilter ref="A1:D1048576" xr:uid="{AFDDA301-E507-4CEA-B648-D07EEDB19C6A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1048576">
+    <sortCondition ref="B1:B1048576"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4DE59296-9C66-4043-8D81-0B47A4E4D022}" name="Site IDs after depth filtering"/>
+    <tableColumn id="2" xr3:uid="{D25C7B6E-2719-4651-A9FA-9CF98A81C9CF}" name="OR site ranks"/>
+    <tableColumn id="3" xr3:uid="{9F1E5E75-CFD3-4089-B7AD-D05B74BB2A99}" name="TOPSIS site ranks"/>
+    <tableColumn id="4" xr3:uid="{04992053-DEA3-4580-938A-82B85E58ED52}" name="VIKOR site ranks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,73 +670,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="B4">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>46</v>
+        <v>226</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -746,874 +754,877 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>49</v>
+        <v>226</v>
       </c>
       <c r="B6">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>54</v>
+        <v>229</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>56</v>
+        <v>241</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="B9">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>76</v>
+        <v>229</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="B12">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="B13">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="B14">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>116</v>
+        <v>263</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="B17">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="B18">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>136</v>
+        <v>218</v>
       </c>
       <c r="B19">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="D19">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D20">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="B21">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="B23">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C23">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="D23">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>166</v>
+        <v>76</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D24">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="B25">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B26">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D27">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D29">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="B30">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C30">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="B31">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D31">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B32">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C32">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D32">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B34">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C34">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D34">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>204</v>
+        <v>299</v>
       </c>
       <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>33</v>
+      </c>
+      <c r="D36">
         <v>18</v>
-      </c>
-      <c r="C36">
-        <v>16</v>
-      </c>
-      <c r="D36">
-        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>208</v>
+        <v>286</v>
       </c>
       <c r="B37">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C37">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D37">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>216</v>
+        <v>281</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="B39">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D39">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="B40">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C40">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="D40">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="B42">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D42">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>226</v>
+        <v>39</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="B45">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C45">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D45">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D46">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B48">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C48">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D48">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B49">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C49">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D49">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B50">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C50">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D50">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B51">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C51">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>239</v>
+        <v>85</v>
       </c>
       <c r="B52">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C52">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D52">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="B53">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C53">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D53">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>241</v>
+        <v>87</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>245</v>
+        <v>199</v>
       </c>
       <c r="B55">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C55">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D55">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B56">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>50</v>
+      </c>
+      <c r="D56">
         <v>40</v>
-      </c>
-      <c r="C56">
-        <v>48</v>
-      </c>
-      <c r="D56">
-        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="B57">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C57">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D57">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>252</v>
+        <v>136</v>
       </c>
       <c r="B58">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C58">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D58">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>253</v>
+        <v>101</v>
       </c>
       <c r="B59">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C59">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D59">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>254</v>
+        <v>220</v>
       </c>
       <c r="B60">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C61">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D61">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62">
-        <v>260</v>
+        <v>157</v>
       </c>
       <c r="B62">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C62">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D62">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>263</v>
+        <v>49</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C63">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D63">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>270</v>
+        <v>133</v>
       </c>
       <c r="B64">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C64">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D64">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>281</v>
+        <v>75</v>
       </c>
       <c r="B65">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C65">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D65">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="B66">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C66">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D66">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>299</v>
+        <v>236</v>
       </c>
       <c r="B67">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C67">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D67">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>